<commit_message>
first stage changed, POR for segment controller
</commit_message>
<xml_diff>
--- a/kicad/cdm324_v2/prod_files/cdm324_v2_bom.xlsx
+++ b/kicad/cdm324_v2/prod_files/cdm324_v2_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\limpkin\Dropbox\Projets\cdm324_v2\kicad\current_rev\prod_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\limpkin\Dropbox\Projets\cdm324_fft\kicad\cdm324_v2\prod_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{54AB52DE-64D6-44D3-88D2-CFDFD99F4158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1420C5E-464B-469E-B498-15E20107EBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240"/>
+    <workbookView xWindow="10545" yWindow="6135" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cdm324_v2_bom_digikey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
   <si>
     <t>Qty</t>
   </si>
@@ -52,15 +52,6 @@
     <t>C4</t>
   </si>
   <si>
-    <t>200p</t>
-  </si>
-  <si>
-    <t>CL10C201JB8NNNC</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10C201JB8NNNC/1276-2222-1-ND/3890308</t>
-  </si>
-  <si>
     <t>C2, C6, C7, C8, C12, C14, C15, C16, C18</t>
   </si>
   <si>
@@ -154,9 +145,6 @@
     <t>https://www.digikey.com/en/products/detail/yageo/RC0402JR-0775RL/726505</t>
   </si>
   <si>
-    <t>R3, R5, R6</t>
-  </si>
-  <si>
     <t>130k</t>
   </si>
   <si>
@@ -268,9 +256,6 @@
     <t>0603</t>
   </si>
   <si>
-    <t>C107080</t>
-  </si>
-  <si>
     <t>0402</t>
   </si>
   <si>
@@ -317,12 +302,39 @@
   </si>
   <si>
     <t>Alternative LCSC part number</t>
+  </si>
+  <si>
+    <t>R5, R6</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>CC0603JRNPO9BN270</t>
+  </si>
+  <si>
+    <t>C107045</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CC0603JRNPO9BN270/302797</t>
+  </si>
+  <si>
+    <t>27pF</t>
+  </si>
+  <si>
+    <t>RC0603FR-07620KL</t>
+  </si>
+  <si>
+    <t>620k</t>
+  </si>
+  <si>
+    <t>C68737</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1168,35 +1180,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.15234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.3828125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.3828125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.3828125" customWidth="1"/>
-    <col min="9" max="9" width="104.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="104.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1208,16 +1220,16 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1237,16 +1249,16 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1257,25 +1269,25 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1283,28 +1295,28 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1312,28 +1324,28 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1341,25 +1353,28 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1367,25 +1382,25 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1393,25 +1408,25 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1419,28 +1434,28 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
       <c r="G9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1448,57 +1463,57 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>75</v>
       </c>
       <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
       <c r="G10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1506,25 +1521,25 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>53</v>
-      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1532,25 +1547,25 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1558,25 +1573,25 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1584,25 +1599,25 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" t="s">
-        <v>88</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>67</v>
-      </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1610,25 +1625,25 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1636,33 +1651,59 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I9" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2"/>
-    <hyperlink ref="I3" r:id="rId3"/>
-    <hyperlink ref="I4" r:id="rId4"/>
-    <hyperlink ref="I5" r:id="rId5"/>
-    <hyperlink ref="I6" r:id="rId6"/>
-    <hyperlink ref="I7" r:id="rId7"/>
-    <hyperlink ref="I8" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
-    <hyperlink ref="I11" r:id="rId10"/>
-    <hyperlink ref="I12" r:id="rId11"/>
-    <hyperlink ref="I13" r:id="rId12"/>
-    <hyperlink ref="I14" r:id="rId13"/>
-    <hyperlink ref="I15" r:id="rId14"/>
-    <hyperlink ref="I16" r:id="rId15"/>
-    <hyperlink ref="I17" r:id="rId16"/>
+    <hyperlink ref="I9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="I11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="I13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="I14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="I15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="I17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="I3" r:id="rId16" xr:uid="{360138F2-0FC2-44F8-8212-DC71977FB862}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>